<commit_message>
Update RLQSO sample with radio-galaxies
</commit_message>
<xml_diff>
--- a/RLQSO/radio_sources.xlsx
+++ b/RLQSO/radio_sources.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tomas Soltinsky\Documents\astrophysics\literature\RLQSO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A52D6FC8-1566-4387-AD1F-09B0A2C0DDC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE23B046-593C-4E80-A1E5-CAB3087A355B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="540" windowWidth="18564" windowHeight="11700" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1488" yWindow="1296" windowWidth="20004" windowHeight="10356" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hárok1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="108">
   <si>
     <t>name</t>
   </si>
@@ -339,6 +339,27 @@
   </si>
   <si>
     <t>Banados+2024</t>
+  </si>
+  <si>
+    <t>Until 2014 included</t>
+  </si>
+  <si>
+    <t>Until 2015 included</t>
+  </si>
+  <si>
+    <t>J0856+0224</t>
+  </si>
+  <si>
+    <t>Drouart+20</t>
+  </si>
+  <si>
+    <t>J1530+1049</t>
+  </si>
+  <si>
+    <t>Saxena+18</t>
+  </si>
+  <si>
+    <t>RLQSO until 2020</t>
   </si>
 </sst>
 </file>
@@ -720,10 +741,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z35"/>
+  <dimension ref="A1:Z37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q12" sqref="Q12"/>
+    <sheetView tabSelected="1" topLeftCell="T1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Z12" sqref="Z12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -869,7 +890,7 @@
       </c>
       <c r="X2">
         <f>COUNT(B2:B102)</f>
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="Y2">
         <f>COUNTIF(B2:B102,"&gt;=6")</f>
@@ -877,7 +898,7 @@
       </c>
       <c r="Z2">
         <f>COUNTIF(Q2:Q102,"&gt;0")</f>
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.3">
@@ -918,12 +939,12 @@
         <v>93</v>
       </c>
       <c r="X3">
-        <f>COUNTA(R2,R3,R4,R5,R12,R14,S21,S22,S23,R31,R32,R35)</f>
-        <v>12</v>
+        <f>COUNTA(R2,R3,R4,R5,R14,S21,S22,S23,R31,R32,R35,R36,R37)</f>
+        <v>13</v>
       </c>
       <c r="Y3">
-        <f>COUNTA(R12,S22,R31,R32)</f>
-        <v>4</v>
+        <f>COUNTA(S22,R31,R32)</f>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.3">
@@ -962,11 +983,11 @@
       </c>
       <c r="X4">
         <f>X2/X3</f>
-        <v>2.8333333333333335</v>
+        <v>2.7692307692307692</v>
       </c>
       <c r="Y4">
         <f>Y2/Y3</f>
-        <v>3.75</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.3">
@@ -1027,6 +1048,17 @@
       <c r="V5" t="s">
         <v>74</v>
       </c>
+      <c r="W5" t="s">
+        <v>101</v>
+      </c>
+      <c r="X5">
+        <f>COUNTA(R14,S21,S2,R32,R35,R31)</f>
+        <v>6</v>
+      </c>
+      <c r="Y5">
+        <f>COUNTA(R31,R32)</f>
+        <v>2</v>
+      </c>
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
@@ -1084,6 +1116,14 @@
       <c r="V6" t="s">
         <v>76</v>
       </c>
+      <c r="X6">
+        <f>X2/X5</f>
+        <v>6</v>
+      </c>
+      <c r="Y6">
+        <f>Y2/Y5</f>
+        <v>7.5</v>
+      </c>
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
@@ -1104,6 +1144,9 @@
       <c r="F7">
         <v>4.6580000000000004</v>
       </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
       <c r="H7">
         <v>3.226</v>
       </c>
@@ -1166,6 +1209,9 @@
       <c r="F8">
         <v>0.24099999999999999</v>
       </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
       <c r="H8">
         <v>0.438</v>
       </c>
@@ -1189,6 +1235,17 @@
       </c>
       <c r="V8" t="s">
         <v>75</v>
+      </c>
+      <c r="W8" t="s">
+        <v>102</v>
+      </c>
+      <c r="X8">
+        <f>COUNTA(R2:R4,R14,S21,R31,R32,R35)</f>
+        <v>8</v>
+      </c>
+      <c r="Y8">
+        <f>COUNTA(R31,R32)</f>
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:26" x14ac:dyDescent="0.3">
@@ -1225,6 +1282,14 @@
       <c r="V9" t="s">
         <v>74</v>
       </c>
+      <c r="X9">
+        <f>X2/X8</f>
+        <v>4.5</v>
+      </c>
+      <c r="Y9">
+        <f>Y3/Y8</f>
+        <v>1.5</v>
+      </c>
     </row>
     <row r="10" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
@@ -1378,6 +1443,17 @@
       <c r="V12" t="s">
         <v>73</v>
       </c>
+      <c r="W12" t="s">
+        <v>107</v>
+      </c>
+      <c r="X12">
+        <f>COUNT(B2:B102)-COUNT(B36,B37)</f>
+        <v>34</v>
+      </c>
+      <c r="Y12">
+        <f>COUNTIF(B2:B112,"&gt;=6")</f>
+        <v>15</v>
+      </c>
     </row>
     <row r="13" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
@@ -1422,6 +1498,14 @@
       <c r="R13" t="s">
         <v>41</v>
       </c>
+      <c r="X13">
+        <f>COUNTA(R2,R3,R4,R5,R14,S21,S22,S23,R31,R32,R35)</f>
+        <v>11</v>
+      </c>
+      <c r="Y13">
+        <f>COUNTA(S22,R31,R32)</f>
+        <v>3</v>
+      </c>
     </row>
     <row r="14" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
@@ -1465,6 +1549,14 @@
       </c>
       <c r="S14" s="2" t="s">
         <v>44</v>
+      </c>
+      <c r="X14">
+        <f>X12/X13</f>
+        <v>3.0909090909090908</v>
+      </c>
+      <c r="Y14">
+        <f>Y12/Y13</f>
+        <v>5</v>
       </c>
     </row>
     <row r="15" spans="1:26" x14ac:dyDescent="0.3">
@@ -2337,6 +2429,76 @@
       </c>
       <c r="S35" s="2" t="s">
         <v>44</v>
+      </c>
+    </row>
+    <row r="36" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>103</v>
+      </c>
+      <c r="B36" s="1">
+        <v>5.55</v>
+      </c>
+      <c r="F36">
+        <v>899.82</v>
+      </c>
+      <c r="G36">
+        <v>0</v>
+      </c>
+      <c r="H36" s="1">
+        <v>86.5</v>
+      </c>
+      <c r="I36">
+        <v>0</v>
+      </c>
+      <c r="K36">
+        <v>-1.18</v>
+      </c>
+      <c r="L36">
+        <v>0</v>
+      </c>
+      <c r="M36">
+        <v>0</v>
+      </c>
+      <c r="P36">
+        <v>8.9369999999999994</v>
+      </c>
+      <c r="Q36">
+        <v>2.4</v>
+      </c>
+      <c r="R36" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="37" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>105</v>
+      </c>
+      <c r="B37" s="1">
+        <v>5.72</v>
+      </c>
+      <c r="F37">
+        <v>174.88</v>
+      </c>
+      <c r="G37">
+        <v>0</v>
+      </c>
+      <c r="H37" s="1">
+        <v>7.5</v>
+      </c>
+      <c r="I37">
+        <v>0</v>
+      </c>
+      <c r="K37">
+        <v>-1.4</v>
+      </c>
+      <c r="P37">
+        <v>15.513999999999999</v>
+      </c>
+      <c r="Q37">
+        <v>10.824999999999999</v>
+      </c>
+      <c r="R37" t="s">
+        <v>106</v>
       </c>
     </row>
   </sheetData>

</xml_diff>